<commit_message>
set all key values to lowercase
</commit_message>
<xml_diff>
--- a/Bizagi/simulation_metrics.xlsx
+++ b/Bizagi/simulation_metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Data\Bizagi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:9_{9819BCFB-CE32-4F9C-A9CD-BCC0A7554E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB0C58BE-D606-4938-90B4-17119AD43523}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:9_{9819BCFB-CE32-4F9C-A9CD-BCC0A7554E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FFA39C-07DA-4D38-A661-22DC4899A92D}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="4185" windowWidth="25815" windowHeight="12030" xr2:uid="{1DFEDFA4-C2BE-44EB-BC93-19389BFEE2AD}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>Monthly</t>
   </si>
   <si>
-    <t>Start event</t>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -968,7 +968,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1139,10 +1139,10 @@
         <v>22</v>
       </c>
       <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
         <v>10</v>
-      </c>
-      <c r="K8">
-        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>